<commit_message>
added documentation for icdf
</commit_message>
<xml_diff>
--- a/results/2013.09.03_heston_loc_comparison/heston_loc.xlsx
+++ b/results/2013.09.03_heston_loc_comparison/heston_loc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>finance.webpricer</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Heston</t>
-  </si>
-  <si>
-    <t>Box Muller</t>
   </si>
   <si>
     <t>RNG</t>
@@ -659,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -671,20 +668,20 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -693,10 +690,10 @@
       </c>
       <c r="B6" s="6">
         <f>SUM(B7:B10)</f>
-        <v>335</v>
+        <v>415</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="6">
         <f>SUM(E7)</f>
@@ -711,7 +708,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2">
         <f>30+180</f>
@@ -720,10 +717,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2">
-        <v>45</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -736,7 +733,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2">
         <v>110</v>
@@ -744,14 +741,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6">
         <f>SUM(B13:B17)</f>
         <v>540</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="6">
         <f>SUM(E13:E14)</f>
@@ -760,14 +757,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <f>50+40</f>
         <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2">
         <v>40</v>
@@ -775,13 +772,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2">
         <v>110</v>
@@ -789,7 +786,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>230</v>
@@ -797,7 +794,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>70</v>
@@ -805,7 +802,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>110</v>
@@ -815,7 +812,7 @@
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -907,7 +904,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2">
         <f>SUM(D30:F30)</f>
@@ -933,12 +930,12 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="2">
         <f>SUM(D34)</f>
@@ -950,27 +947,27 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2">
         <f>SUM(D37:P37,D39:J39)</f>
@@ -997,25 +994,25 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J38" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1043,12 +1040,12 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D41" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" ref="B42" si="0">SUM(D42:P42)</f>
@@ -1060,34 +1057,34 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="6">
         <f>SUM(B25:B42)</f>
         <v>3705</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,23 +1095,23 @@
         <v>250</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2">
         <v>180</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2">
         <v>900</v>
@@ -1122,14 +1119,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B56" s="6">
         <f>SUM(B52:B54)</f>
         <v>1330</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1151,7 +1148,7 @@
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -1161,10 +1158,10 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E68" s="2">
         <v>300</v>
@@ -1172,7 +1169,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D70" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>20</v>
@@ -1181,18 +1178,18 @@
         <v>18</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H70" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="2">
         <f>SUM(D71:P71,D73:J73)</f>
@@ -1219,25 +1216,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D72" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H72" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -1265,12 +1262,12 @@
     </row>
     <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2">
         <f>180+40+50+150+470+110</f>
@@ -1279,7 +1276,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="2">
         <v>310</v>
@@ -1287,7 +1284,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="2">
         <f>160+80+90</f>
@@ -1296,7 +1293,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="2">
         <v>300</v>
@@ -1304,24 +1301,24 @@
     </row>
     <row r="83" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B83" s="6">
         <f>SUM(B71,B78:B81,E68)</f>
         <v>5280</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88" s="2">
         <v>1200</v>
@@ -1329,7 +1326,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" s="2">
         <v>400</v>
@@ -1337,7 +1334,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="2">
         <v>680</v>
@@ -1353,7 +1350,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" s="2">
         <v>3300</v>
@@ -1361,14 +1358,14 @@
     </row>
     <row r="94" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B94" s="6">
         <f>SUM(B88:B92)</f>
         <v>7870</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>